<commit_message>
updated code for frame work
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{91183FE8-4831-4CF0-95FC-9E7BE64C0831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7CEC2CD5-56C3-4037-983C-77E08698283E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0D6212A0-BA21-4A92-89C9-8D046F230113}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0D6212A0-BA21-4A92-89C9-8D046F230113}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
@@ -13,19 +13,10 @@
     <sheet name="trialnow" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:U15"/>
+  <oleSize ref="A1:I17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -548,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DA7413-B492-4F1F-94E8-6BD95E4A2285}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>